<commit_message>
Avance de Front, conexión con Back.
</commit_message>
<xml_diff>
--- a/documentacion/Diseño BD.xlsx
+++ b/documentacion/Diseño BD.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Desarrollo\desarrollador\Pautas y diseños\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Desarrollo\desarrollador\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D8E4E755-4D0A-42BB-B782-5F0FF776717B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5589B221-AD1E-4F67-944B-152E29832E6F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{2A50DBC5-228F-4775-ACB4-BA2755C6E406}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7635" xr2:uid="{2A50DBC5-228F-4775-ACB4-BA2755C6E406}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Estructura" sheetId="1" r:id="rId1"/>
+    <sheet name="Datos" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="38">
   <si>
     <t>tb_sitio</t>
   </si>
@@ -194,14 +195,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="20% - Énfasis1" xfId="1" builtinId="30"/>
@@ -247,8 +249,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1BF930DD-1196-4302-9040-F2F2D04C45D4}" name="Tabla3" displayName="Tabla3" ref="A37:D49" totalsRowShown="0">
-  <autoFilter ref="A37:D49" xr:uid="{606AED7D-BD03-4C47-862B-B330AD77223A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1BF930DD-1196-4302-9040-F2F2D04C45D4}" name="Tabla3" displayName="Tabla3" ref="A37:D50" totalsRowShown="0">
+  <autoFilter ref="A37:D50" xr:uid="{606AED7D-BD03-4C47-862B-B330AD77223A}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{E6E43FB0-88D2-49C4-BA20-FFEC2D5391C4}" name="CAMPO"/>
     <tableColumn id="2" xr3:uid="{1D778950-FD4F-4868-B59A-7F74FB035D57}" name="TIPO"/>
@@ -582,10 +584,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C557126E-5E27-4754-85E5-E3E6C5298F16}">
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,9 +602,9 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -668,12 +670,12 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -739,12 +741,12 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -799,12 +801,12 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -870,12 +872,12 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+      <c r="A36" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -977,6 +979,9 @@
       <c r="B46" t="s">
         <v>13</v>
       </c>
+      <c r="D46" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
@@ -985,26 +990,41 @@
       <c r="B47" t="s">
         <v>13</v>
       </c>
+      <c r="D47" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>16</v>
+      </c>
+      <c r="B48" t="s">
+        <v>20</v>
+      </c>
+      <c r="D48" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>7</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>11</v>
       </c>
-      <c r="C48">
+      <c r="C49">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="D49" s="3"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>8</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>12</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C50" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1017,12 +1037,25 @@
     <mergeCell ref="A19:D19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="5">
-    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2281208C-C1C6-49F6-ADD1-39355910D1F5}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>